<commit_message>
7 Dec , Added Comments,Aligned Code and organised
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anike\PycharmProjects\Automation_API_Extract\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1E4A00-F935-41DE-A81F-508749297FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EE97F5-1C3B-42C7-B455-E3F37CB91B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1695" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datasheet" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <t>Share</t>
   </si>
   <si>
-    <t>Tata Motors Ltd</t>
+    <t>TCS</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,7 +411,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
         <f ca="1">_xlfn.CONCAT("ryan",RANDBETWEEN(10,99),"@gmail.com")</f>
-        <v>ryan71@gmail.com</v>
+        <v>ryan66@gmail.com</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>

</xml_diff>